<commit_message>
lesson 3&4 作业统计 (#83)
</commit_message>
<xml_diff>
--- a/data/rating/2019_assignments_rating.xlsx
+++ b/data/rating/2019_assignments_rating.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13911\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AI课程Markdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E3B7C5-19FB-4740-9B6B-7C1D6C058320}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BB44087-EFD4-4707-A98E-2E33F2DEC14A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1815" windowWidth="23040" windowHeight="12195" xr2:uid="{B8E76769-7D0E-4623-87D1-61E9A2044D09}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>序号</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -163,6 +162,18 @@
   </si>
   <si>
     <t>lesson02</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>lesson03</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -289,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{D659C700-F8BF-49B1-B6F3-8B1C83EF3063}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -306,7 +317,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -602,9 +613,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D410068-B893-4195-8EAD-430B37C7C3F8}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -615,7 +626,7 @@
     <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,10 +643,13 @@
         <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -651,12 +665,15 @@
       <c r="E2" s="3">
         <v>100</v>
       </c>
-      <c r="F2" s="1">
-        <f>E2</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="3">
+        <v>100</v>
+      </c>
+      <c r="G2" s="1">
+        <f>$E2+$F2</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -672,12 +689,15 @@
       <c r="E3" s="3">
         <v>100</v>
       </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F22" si="0">E3</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="1" t="e">
+        <f>$E3+$F3</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -693,12 +713,15 @@
       <c r="E4" s="3">
         <v>90</v>
       </c>
-      <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="3">
+        <v>80</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ref="G4:G22" si="0">$E4+$F4</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -714,12 +737,15 @@
       <c r="E5" s="3">
         <v>90</v>
       </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="3">
+        <v>80</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -735,12 +761,15 @@
       <c r="E6" s="3">
         <v>90</v>
       </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="3">
+        <v>40</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -756,12 +785,14 @@
       <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F7" s="3">
+        <v>60</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -777,12 +808,15 @@
       <c r="E8" s="3">
         <v>90</v>
       </c>
-      <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F8" s="3">
+        <v>80</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -798,12 +832,15 @@
       <c r="E9" s="3">
         <v>90</v>
       </c>
-      <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F9" s="3">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -819,12 +856,15 @@
       <c r="E10" s="3">
         <v>90</v>
       </c>
-      <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F10" s="3">
+        <v>80</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -840,12 +880,15 @@
       <c r="E11" s="3">
         <v>80</v>
       </c>
-      <c r="F11" s="1">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="3">
+        <v>60</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -861,12 +904,15 @@
       <c r="E12" s="3">
         <v>100</v>
       </c>
-      <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="3">
+        <v>80</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -882,12 +928,15 @@
       <c r="E13" s="3">
         <v>100</v>
       </c>
-      <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="3">
+        <v>60</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -903,12 +952,15 @@
       <c r="E14" s="3">
         <v>90</v>
       </c>
-      <c r="F14" s="1">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="3">
+        <v>80</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -924,12 +976,15 @@
       <c r="E15" s="3">
         <v>80</v>
       </c>
-      <c r="F15" s="1">
-        <f t="shared" si="0"/>
+      <c r="F15" s="3">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -945,12 +1000,14 @@
       <c r="E16" s="3">
         <v>90</v>
       </c>
-      <c r="F16" s="1">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -966,12 +1023,15 @@
       <c r="E17" s="3">
         <v>100</v>
       </c>
-      <c r="F17" s="1">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F17" s="3">
+        <v>100</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -987,12 +1047,15 @@
       <c r="E18" s="3">
         <v>100</v>
       </c>
-      <c r="F18" s="1">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F18" s="3">
+        <v>100</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>19</v>
       </c>
@@ -1008,12 +1071,15 @@
       <c r="E19" s="3">
         <v>100</v>
       </c>
-      <c r="F19" s="1">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="3">
+        <v>100</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>20</v>
       </c>
@@ -1029,12 +1095,15 @@
       <c r="E20" s="3">
         <v>90</v>
       </c>
-      <c r="F20" s="1">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="3">
+        <v>100</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="0"/>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>21</v>
       </c>
@@ -1050,12 +1119,14 @@
       <c r="E21" s="3">
         <v>80</v>
       </c>
-      <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>22</v>
       </c>
@@ -1071,9 +1142,12 @@
       <c r="E22" s="3">
         <v>80</v>
       </c>
-      <c r="F22" s="1">
-        <f t="shared" si="0"/>
-        <v>80</v>
+      <c r="F22" s="3">
+        <v>100</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>